<commit_message>
recurrencedated is returning 2 things
</commit_message>
<xml_diff>
--- a/D:\test excel\doubletest.xlsx
+++ b/D:\test excel\doubletest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoeking/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4C02C3-B3C2-F645-8BAF-B76B11DB4181}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC1ED57-03A4-C049-A3D8-E5D715528A5C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="680" windowWidth="24000" windowHeight="10620" xr2:uid="{893D501D-C101-984A-9105-6A5D73813DB5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>AB191623305</t>
   </si>
@@ -72,18 +72,6 @@
     </r>
   </si>
   <si>
-    <t>2.22.21.EOM1.</t>
-  </si>
-  <si>
-    <t>AB188009867</t>
-  </si>
-  <si>
-    <t>2021-01-06 08:21:37</t>
-  </si>
-  <si>
-    <t>Braunfundraiser.nonDD.1.6.20.</t>
-  </si>
-  <si>
     <t>Receipt ID</t>
   </si>
   <si>
@@ -127,6 +115,9 @@
   </si>
   <si>
     <t>Reference Code</t>
+  </si>
+  <si>
+    <t>Email45</t>
   </si>
 </sst>
 </file>
@@ -505,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04395FC3-9BB2-5640-BE44-6EFCE76CAC59}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -518,49 +509,49 @@
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -605,58 +596,12 @@
         <v>5025523990</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="4">
-        <v>50</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4">
-        <v>1</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K3" s="4">
-        <v>40207</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N3" s="4">
-        <v>5025523990</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M3" r:id="rId1" xr:uid="{CFF09C6D-8282-2045-813F-8F1644B61744}"/>
-    <hyperlink ref="M2" r:id="rId2" xr:uid="{2214E67D-333D-5B42-A93D-FC46608E83C8}"/>
+    <hyperlink ref="M2" r:id="rId1" xr:uid="{2214E67D-333D-5B42-A93D-FC46608E83C8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
recurrendated is fi fixed
</commit_message>
<xml_diff>
--- a/D:\test excel\doubletest.xlsx
+++ b/D:\test excel\doubletest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoeking/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC1ED57-03A4-C049-A3D8-E5D715528A5C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B083BA-668D-DE4D-A89D-500C0A63D68A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="680" windowWidth="24000" windowHeight="10620" xr2:uid="{893D501D-C101-984A-9105-6A5D73813DB5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t>AB191623305</t>
   </si>
@@ -72,6 +72,12 @@
     </r>
   </si>
   <si>
+    <t>AB188009867</t>
+  </si>
+  <si>
+    <t>2021-01-06 08:21:37</t>
+  </si>
+  <si>
     <t>Receipt ID</t>
   </si>
   <si>
@@ -118,6 +124,12 @@
   </si>
   <si>
     <t>Email45</t>
+  </si>
+  <si>
+    <t>AB288009867</t>
+  </si>
+  <si>
+    <t>2021-02-06 08:21:37</t>
   </si>
 </sst>
 </file>
@@ -496,62 +508,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04395FC3-9BB2-5640-BE44-6EFCE76CAC59}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="5"/>
+    <col min="1" max="1" width="10.83203125" style="5"/>
+    <col min="2" max="2" width="18.33203125" style="5" customWidth="1"/>
+    <col min="3" max="13" width="10.83203125" style="5"/>
+    <col min="14" max="14" width="20" style="5" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -596,12 +612,104 @@
         <v>5025523990</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4">
+        <v>50</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="4">
+        <v>40207</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" s="4">
+        <v>5025523990</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="4">
+        <v>50</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="4">
+        <v>40207</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="4">
+        <v>5025523990</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="M2" r:id="rId1" xr:uid="{2214E67D-333D-5B42-A93D-FC46608E83C8}"/>
+    <hyperlink ref="M3" r:id="rId2" xr:uid="{150891AC-7FB6-6046-A2C2-E74A89787B95}"/>
+    <hyperlink ref="M4" r:id="rId3" xr:uid="{67429B3C-0186-E64D-90E7-8B41D9A0031C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>